<commit_message>
Modified test methods in merchant portal
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_Merchant.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_Merchant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COYNIv_2.3_Merchant\17-Apr-2023(Merchant)\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EFF7A7-74FF-4392-8156-FE38AF63D0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BBEF35-5DED-4573-B350-D7AE7B75BD4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2802,8 +2801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4575,7 +4574,7 @@
         <v>114</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>365</v>
+        <v>237</v>
       </c>
       <c r="C61" t="s">
         <v>115</v>

</xml_diff>

<commit_message>
Modified test methods of Business token account feature in Merchant portal
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_Merchant.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_Merchant.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COYNIv_2.3_Merchant\17-Apr-2023(Merchant)\coyni-automation\Mobile\coyni_mobile\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COYNIv_2.3_Merchant\19-apr-2023(Merchant)\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BBEF35-5DED-4573-B350-D7AE7B75BD4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072A91F2-8B80-40A9-A7EA-F203AF1B9324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2801,8 +2801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4690,7 +4690,7 @@
         <v>122</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>365</v>
+        <v>237</v>
       </c>
       <c r="C65" t="s">
         <v>115</v>
@@ -5560,7 +5560,7 @@
         <v>178</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>237</v>
+        <v>365</v>
       </c>
       <c r="C95" t="s">
         <v>179</v>
@@ -6077,7 +6077,7 @@
         <v>10</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G112" s="5" t="s">
         <v>337</v>
@@ -6787,7 +6787,7 @@
       <c r="N134" s="11"/>
     </row>
     <row r="135" spans="1:14" ht="135" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="A135" s="12" t="s">
         <v>277</v>
       </c>
       <c r="B135" s="13" t="s">

</xml_diff>

<commit_message>
Developed the test methods for processing fee
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_Merchant.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_Merchant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COYNIv_2.3_Merchant\19-apr-2023(Merchant)\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072A91F2-8B80-40A9-A7EA-F203AF1B9324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687B8FAE-E096-4AF7-944F-D933151E95DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2801,8 +2801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5560,7 +5560,7 @@
         <v>178</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>365</v>
+        <v>237</v>
       </c>
       <c r="C95" t="s">
         <v>179</v>
@@ -5705,7 +5705,7 @@
         <v>189</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>237</v>
+        <v>365</v>
       </c>
       <c r="C100" t="s">
         <v>190</v>
@@ -5714,7 +5714,7 @@
         <v>12</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>13</v>
@@ -6077,7 +6077,7 @@
         <v>10</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G112" s="5" t="s">
         <v>337</v>
@@ -6196,7 +6196,7 @@
         <v>12</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F116" s="6" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Developed the test methods for Sale order token transaction
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_Merchant.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_Merchant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COYNIv_2.3_Merchant\19-apr-2023(Merchant)\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687B8FAE-E096-4AF7-944F-D933151E95DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D32943-0699-4F6D-82BC-CDB5C79028F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="373">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1635,17 +1635,6 @@
   </si>
   <si>
     <t xml:space="preserve">verify All the states </t>
-  </si>
-  <si>
-    <t>coyni_mobile_merchant.tests.MerchantProfileTest,
-testVerifyAllStates,
--pcardNumber,
--pcardExp,
--paddressLine1,
--paddressLine2,
--pcity,
--pstate,
--pnameOnCard</t>
   </si>
   <si>
     <t>coyni_mobile_merchant.tests.LoginTest,
@@ -2363,9 +2352,6 @@
 -paddPaymentHeading</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>coyni_mobile_merchant.tests.MerchantProfileTest,
 testChangeEmailWithValidDetails,
 -puserDetailsHeading,
@@ -2414,6 +2400,36 @@
   </si>
   <si>
     <t>verify Login Page Navigations</t>
+  </si>
+  <si>
+    <t>Merchant Payout transaction</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Verify Merhchant Payout transaction</t>
+  </si>
+  <si>
+    <t>coyni_mobile_merchant.tests.DashBoardTest,
+testDashBoardFeeCalculation,
+-plabel,
+-pheading,
+-pamountHeading,
+-pamount,
+-ppin,
+-psaveAlbumToast</t>
+  </si>
+  <si>
+    <t>coyni_mobile_merchant.tests.MerchantProfileTest,
+testVerifyAllStates,
+-pcardNumber,
+-pcardExp,
+-paddressLine1,
+-paddressLine2,
+-pcity,
+-pstates,
+-pnameOnCard</t>
   </si>
 </sst>
 </file>
@@ -2481,7 +2497,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2518,6 +2534,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2799,10 +2816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O135"/>
+  <dimension ref="A1:O136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2873,7 +2890,7 @@
     </row>
     <row r="2" spans="1:15" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>237</v>
@@ -2891,10 +2908,10 @@
         <v>10</v>
       </c>
       <c r="G2" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>309</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>310</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -2939,7 +2956,7 @@
     </row>
     <row r="4" spans="1:15" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>237</v>
@@ -2960,7 +2977,7 @@
         <v>26</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -2993,7 +3010,7 @@
         <v>227</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I5" s="11" t="s">
         <v>229</v>
@@ -3005,7 +3022,7 @@
         <v>231</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="2"/>
@@ -3013,7 +3030,7 @@
     </row>
     <row r="6" spans="1:15" ht="330" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>237</v>
@@ -3034,7 +3051,7 @@
         <v>227</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -3067,7 +3084,7 @@
         <v>11</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -3124,7 +3141,7 @@
     </row>
     <row r="10" spans="1:15" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>237</v>
@@ -3145,7 +3162,7 @@
         <v>11</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="210" x14ac:dyDescent="0.25">
@@ -3174,7 +3191,7 @@
         <v>18</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="210" x14ac:dyDescent="0.25">
@@ -3356,7 +3373,7 @@
         <v>30</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3408,7 +3425,7 @@
         <v>41</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -3434,7 +3451,7 @@
         <v>41</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3486,7 +3503,7 @@
         <v>47</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>48</v>
@@ -3515,7 +3532,7 @@
         <v>47</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I24" s="7" t="s">
         <v>50</v>
@@ -3523,7 +3540,7 @@
     </row>
     <row r="25" spans="1:10" ht="165.75" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>237</v>
@@ -3544,10 +3561,10 @@
         <v>47</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
@@ -3573,7 +3590,7 @@
         <v>47</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I26" s="7" t="s">
         <v>52</v>
@@ -3602,7 +3619,7 @@
         <v>55</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I27" s="7" t="s">
         <v>217</v>
@@ -3610,7 +3627,7 @@
     </row>
     <row r="28" spans="1:10" ht="153" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>237</v>
@@ -3631,10 +3648,10 @@
         <v>55</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="191.25" x14ac:dyDescent="0.25">
@@ -3660,7 +3677,7 @@
         <v>55</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I29" s="7" t="s">
         <v>58</v>
@@ -3689,7 +3706,7 @@
         <v>55</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I30" s="7" t="s">
         <v>60</v>
@@ -3718,7 +3735,7 @@
         <v>63</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I31" s="7" t="s">
         <v>236</v>
@@ -3727,7 +3744,7 @@
     </row>
     <row r="32" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B32" s="13" t="s">
         <v>237</v>
@@ -3748,10 +3765,10 @@
         <v>63</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J32" s="7"/>
     </row>
@@ -3778,7 +3795,7 @@
         <v>63</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I33" s="7" t="s">
         <v>65</v>
@@ -3807,7 +3824,7 @@
         <v>63</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I34" s="7" t="s">
         <v>67</v>
@@ -3836,16 +3853,16 @@
         <v>70</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J35" s="7"/>
     </row>
     <row r="36" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B36" s="13" t="s">
         <v>237</v>
@@ -3866,10 +3883,10 @@
         <v>70</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J36" s="7"/>
     </row>
@@ -3896,7 +3913,7 @@
         <v>70</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I37" s="7" t="s">
         <v>72</v>
@@ -3925,7 +3942,7 @@
         <v>70</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I38" s="7" t="s">
         <v>74</v>
@@ -3954,7 +3971,7 @@
         <v>70</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I39" s="7" t="s">
         <v>253</v>
@@ -3983,7 +4000,7 @@
         <v>77</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I40" s="7" t="s">
         <v>222</v>
@@ -4012,7 +4029,7 @@
         <v>77</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I41" s="7" t="s">
         <v>79</v>
@@ -4041,7 +4058,7 @@
         <v>82</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I42" s="7" t="s">
         <v>83</v>
@@ -4070,10 +4087,10 @@
         <v>82</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
@@ -4099,7 +4116,7 @@
         <v>82</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I44" s="7" t="s">
         <v>213</v>
@@ -4128,7 +4145,7 @@
         <v>82</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I45" s="7" t="s">
         <v>86</v>
@@ -4157,7 +4174,7 @@
         <v>82</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I46" s="7" t="s">
         <v>88</v>
@@ -4165,7 +4182,7 @@
     </row>
     <row r="47" spans="1:10" ht="153" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B47" s="13" t="s">
         <v>237</v>
@@ -4186,10 +4203,10 @@
         <v>82</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
@@ -4215,7 +4232,7 @@
         <v>82</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I48" s="7" t="s">
         <v>214</v>
@@ -4244,7 +4261,7 @@
         <v>82</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I49" s="7" t="s">
         <v>91</v>
@@ -4273,7 +4290,7 @@
         <v>82</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I50" s="7" t="s">
         <v>93</v>
@@ -4302,7 +4319,7 @@
         <v>96</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I51" s="7" t="s">
         <v>97</v>
@@ -4331,7 +4348,7 @@
         <v>96</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I52" s="7" t="s">
         <v>215</v>
@@ -4360,7 +4377,7 @@
         <v>96</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I53" s="7" t="s">
         <v>100</v>
@@ -4389,7 +4406,7 @@
         <v>96</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I54" s="7" t="s">
         <v>102</v>
@@ -4397,7 +4414,7 @@
     </row>
     <row r="55" spans="1:9" ht="165.75" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B55" s="13" t="s">
         <v>237</v>
@@ -4418,10 +4435,10 @@
         <v>96</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="127.5" x14ac:dyDescent="0.25">
@@ -4447,7 +4464,7 @@
         <v>96</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I56" s="7" t="s">
         <v>216</v>
@@ -4476,7 +4493,7 @@
         <v>96</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I57" s="7" t="s">
         <v>105</v>
@@ -4505,7 +4522,7 @@
         <v>96</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I58" s="7" t="s">
         <v>107</v>
@@ -4534,7 +4551,7 @@
         <v>110</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I59" s="7" t="s">
         <v>111</v>
@@ -4563,7 +4580,7 @@
         <v>110</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I60" s="7" t="s">
         <v>113</v>
@@ -4592,7 +4609,7 @@
         <v>116</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I61" s="7" t="s">
         <v>218</v>
@@ -4621,7 +4638,7 @@
         <v>116</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I62" s="7" t="s">
         <v>119</v>
@@ -4650,7 +4667,7 @@
         <v>116</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I63" s="7" t="s">
         <v>121</v>
@@ -4658,7 +4675,7 @@
     </row>
     <row r="64" spans="1:9" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>237</v>
@@ -4676,13 +4693,13 @@
         <v>10</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I64" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="204" x14ac:dyDescent="0.25">
@@ -4708,7 +4725,7 @@
         <v>123</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I65" s="7" t="s">
         <v>219</v>
@@ -4737,7 +4754,7 @@
         <v>123</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I66" s="7" t="s">
         <v>125</v>
@@ -4766,7 +4783,7 @@
         <v>123</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I67" s="7" t="s">
         <v>127</v>
@@ -4795,7 +4812,7 @@
         <v>129</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I68" s="7" t="s">
         <v>220</v>
@@ -4824,7 +4841,7 @@
         <v>132</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I69" s="4" t="s">
         <v>133</v>
@@ -4853,7 +4870,7 @@
         <v>135</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I70" s="4" t="s">
         <v>262</v>
@@ -4882,7 +4899,7 @@
         <v>137</v>
       </c>
       <c r="H71" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I71" s="4" t="s">
         <v>138</v>
@@ -4911,7 +4928,7 @@
         <v>140</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I72" s="4" t="s">
         <v>141</v>
@@ -4940,7 +4957,7 @@
         <v>143</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I73" s="4" t="s">
         <v>144</v>
@@ -4948,7 +4965,7 @@
     </row>
     <row r="74" spans="1:9" ht="102" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B74" s="13" t="s">
         <v>237</v>
@@ -4966,18 +4983,18 @@
         <v>10</v>
       </c>
       <c r="G74" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="H74" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="I74" s="11" t="s">
         <v>362</v>
-      </c>
-      <c r="H74" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="I74" s="11" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="102" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B75" s="13" t="s">
         <v>237</v>
@@ -4995,13 +5012,13 @@
         <v>10</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -5027,7 +5044,7 @@
         <v>147</v>
       </c>
       <c r="H76" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I76" s="4" t="s">
         <v>221</v>
@@ -5056,7 +5073,7 @@
         <v>147</v>
       </c>
       <c r="H77" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I77" s="4" t="s">
         <v>149</v>
@@ -5085,7 +5102,7 @@
         <v>151</v>
       </c>
       <c r="H78" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I78" s="4" t="s">
         <v>152</v>
@@ -5114,7 +5131,7 @@
         <v>155</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I79" s="11" t="s">
         <v>156</v>
@@ -5143,7 +5160,7 @@
         <v>158</v>
       </c>
       <c r="H80" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I80" s="4" t="s">
         <v>159</v>
@@ -5172,7 +5189,7 @@
         <v>160</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I81" s="4" t="s">
         <v>162</v>
@@ -5201,7 +5218,7 @@
         <v>160</v>
       </c>
       <c r="H82" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I82" s="4" t="s">
         <v>249</v>
@@ -5230,7 +5247,7 @@
         <v>160</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I83" s="4" t="s">
         <v>164</v>
@@ -5259,10 +5276,10 @@
         <v>160</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="102" x14ac:dyDescent="0.25">
@@ -5288,7 +5305,7 @@
         <v>166</v>
       </c>
       <c r="H85" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I85" s="4" t="s">
         <v>167</v>
@@ -5317,7 +5334,7 @@
         <v>170</v>
       </c>
       <c r="H86" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I86" s="4" t="s">
         <v>171</v>
@@ -5346,7 +5363,7 @@
         <v>173</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I87" s="4" t="s">
         <v>174</v>
@@ -5375,10 +5392,10 @@
         <v>173</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="102" x14ac:dyDescent="0.25">
@@ -5404,7 +5421,7 @@
         <v>173</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I89" s="4" t="s">
         <v>251</v>
@@ -5433,7 +5450,7 @@
         <v>176</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I90" s="4" t="s">
         <v>244</v>
@@ -5441,7 +5458,7 @@
     </row>
     <row r="91" spans="1:9" ht="102" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B91" s="13" t="s">
         <v>237</v>
@@ -5462,10 +5479,10 @@
         <v>176</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -5491,7 +5508,7 @@
         <v>176</v>
       </c>
       <c r="H92" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I92" s="4" t="s">
         <v>242</v>
@@ -5520,7 +5537,7 @@
         <v>176</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I93" s="4" t="s">
         <v>243</v>
@@ -5549,7 +5566,7 @@
         <v>180</v>
       </c>
       <c r="H94" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I94" s="4" t="s">
         <v>245</v>
@@ -5578,7 +5595,7 @@
         <v>180</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I95" s="4" t="s">
         <v>181</v>
@@ -5607,7 +5624,7 @@
         <v>180</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I96" s="4" t="s">
         <v>183</v>
@@ -5636,7 +5653,7 @@
         <v>180</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I97" s="4" t="s">
         <v>185</v>
@@ -5644,7 +5661,7 @@
     </row>
     <row r="98" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B98" s="13" t="s">
         <v>237</v>
@@ -5665,10 +5682,10 @@
         <v>180</v>
       </c>
       <c r="H98" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I98" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="99" spans="1:11" ht="102" x14ac:dyDescent="0.25">
@@ -5694,7 +5711,7 @@
         <v>187</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I99" s="4" t="s">
         <v>188</v>
@@ -5705,7 +5722,7 @@
         <v>189</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>365</v>
+        <v>237</v>
       </c>
       <c r="C100" t="s">
         <v>190</v>
@@ -5714,7 +5731,7 @@
         <v>12</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>13</v>
@@ -5723,7 +5740,7 @@
         <v>191</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I100" s="4" t="s">
         <v>261</v>
@@ -5746,13 +5763,13 @@
         <v>10</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G101" t="s">
         <v>191</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I101" s="4" t="s">
         <v>193</v>
@@ -5781,7 +5798,7 @@
         <v>191</v>
       </c>
       <c r="H102" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I102" s="4" t="s">
         <v>195</v>
@@ -5789,7 +5806,7 @@
     </row>
     <row r="103" spans="1:11" ht="270" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B103" s="13" t="s">
         <v>237</v>
@@ -5807,13 +5824,13 @@
         <v>10</v>
       </c>
       <c r="G103" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H103" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I103" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J103" s="11"/>
     </row>
@@ -5840,7 +5857,7 @@
         <v>199</v>
       </c>
       <c r="H104" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I104" s="4" t="s">
         <v>210</v>
@@ -5866,21 +5883,21 @@
         <v>13</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H105" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I105" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J105" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="106" spans="1:11" ht="270" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B106" s="13" t="s">
         <v>237</v>
@@ -5898,13 +5915,13 @@
         <v>10</v>
       </c>
       <c r="G106" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H106" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I106" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J106" s="11"/>
     </row>
@@ -5928,13 +5945,13 @@
         <v>13</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H107" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I107" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="108" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
@@ -5957,16 +5974,16 @@
         <v>13</v>
       </c>
       <c r="G108" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H108" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I108" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J108" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="109" spans="1:11" ht="255" x14ac:dyDescent="0.25">
@@ -5989,10 +6006,10 @@
         <v>10</v>
       </c>
       <c r="G109" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H109" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I109" s="4" t="s">
         <v>260</v>
@@ -6002,7 +6019,7 @@
     </row>
     <row r="110" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B110" s="13" t="s">
         <v>237</v>
@@ -6020,19 +6037,19 @@
         <v>13</v>
       </c>
       <c r="G110" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H110" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I110" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="J110" s="11"/>
     </row>
     <row r="111" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B111" s="13" t="s">
         <v>237</v>
@@ -6050,13 +6067,13 @@
         <v>10</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H111" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I111" s="11" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J111" s="11"/>
     </row>
@@ -6080,16 +6097,16 @@
         <v>10</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H112" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I112" s="11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="J112" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="113" spans="1:11" ht="225" x14ac:dyDescent="0.25">
@@ -6112,19 +6129,19 @@
         <v>10</v>
       </c>
       <c r="G113" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H113" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I113" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J113" s="11"/>
     </row>
     <row r="114" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B114" s="13" t="s">
         <v>237</v>
@@ -6142,19 +6159,19 @@
         <v>13</v>
       </c>
       <c r="G114" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H114" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I114" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="J114" s="11"/>
     </row>
     <row r="115" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B115" s="13" t="s">
         <v>237</v>
@@ -6175,10 +6192,10 @@
         <v>203</v>
       </c>
       <c r="H115" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I115" s="11" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="J115" s="11"/>
     </row>
@@ -6202,16 +6219,16 @@
         <v>13</v>
       </c>
       <c r="G116" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I116" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J116" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="117" spans="1:11" ht="255" x14ac:dyDescent="0.25">
@@ -6234,16 +6251,16 @@
         <v>10</v>
       </c>
       <c r="G117" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H117" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I117" s="4" t="s">
         <v>260</v>
       </c>
       <c r="J117" s="11" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K117" s="11" t="s">
         <v>223</v>
@@ -6251,7 +6268,7 @@
     </row>
     <row r="118" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B118" s="13" t="s">
         <v>237</v>
@@ -6269,13 +6286,13 @@
         <v>10</v>
       </c>
       <c r="G118" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H118" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I118" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J118" s="11"/>
       <c r="K118" s="11"/>
@@ -6300,10 +6317,10 @@
         <v>208</v>
       </c>
       <c r="G119" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H119" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I119" s="4" t="s">
         <v>209</v>
@@ -6329,21 +6346,21 @@
         <v>10</v>
       </c>
       <c r="G120" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H120" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I120" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="J120" s="11" t="s">
         <v>347</v>
-      </c>
-      <c r="J120" s="11" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="121" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B121" s="13" t="s">
         <v>237</v>
@@ -6361,13 +6378,13 @@
         <v>10</v>
       </c>
       <c r="G121" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H121" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I121" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J121" s="11"/>
     </row>
@@ -6391,10 +6408,10 @@
         <v>21</v>
       </c>
       <c r="G122" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H122" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I122" s="4" t="s">
         <v>270</v>
@@ -6402,7 +6419,7 @@
     </row>
     <row r="123" spans="1:11" ht="270" x14ac:dyDescent="0.25">
       <c r="A123" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B123" s="13" t="s">
         <v>237</v>
@@ -6420,13 +6437,13 @@
         <v>13</v>
       </c>
       <c r="G123" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H123" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I123" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J123" s="11" t="s">
         <v>224</v>
@@ -6434,7 +6451,7 @@
     </row>
     <row r="124" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B124" s="13" t="s">
         <v>237</v>
@@ -6452,13 +6469,13 @@
         <v>10</v>
       </c>
       <c r="G124" t="s">
+        <v>357</v>
+      </c>
+      <c r="H124" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="I124" s="11" t="s">
         <v>358</v>
-      </c>
-      <c r="H124" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="I124" s="11" t="s">
-        <v>359</v>
       </c>
       <c r="J124" s="11"/>
     </row>
@@ -6482,10 +6499,10 @@
         <v>169</v>
       </c>
       <c r="G125" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H125" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I125" s="4" t="s">
         <v>260</v>
@@ -6511,13 +6528,13 @@
         <v>10</v>
       </c>
       <c r="G126" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H126" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I126" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="127" spans="1:11" ht="225" x14ac:dyDescent="0.25">
@@ -6540,13 +6557,13 @@
         <v>169</v>
       </c>
       <c r="G127" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H127" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I127" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="128" spans="1:11" ht="102" x14ac:dyDescent="0.25">
@@ -6569,13 +6586,13 @@
         <v>10</v>
       </c>
       <c r="G128" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H128" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I128" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J128" s="11"/>
     </row>
@@ -6599,10 +6616,10 @@
         <v>13</v>
       </c>
       <c r="G129" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H129" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I129" s="4" t="s">
         <v>271</v>
@@ -6629,13 +6646,13 @@
         <v>10</v>
       </c>
       <c r="G130" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H130" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I130" s="11" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="131" spans="1:14" ht="102" x14ac:dyDescent="0.25">
@@ -6658,10 +6675,10 @@
         <v>10</v>
       </c>
       <c r="G131" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H131" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I131" s="11" t="s">
         <v>255</v>
@@ -6669,7 +6686,7 @@
     </row>
     <row r="132" spans="1:14" ht="255" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B132" s="13" t="s">
         <v>237</v>
@@ -6687,13 +6704,13 @@
         <v>10</v>
       </c>
       <c r="G132" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H132" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I132" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J132" s="11" t="s">
         <v>230</v>
@@ -6702,12 +6719,12 @@
         <v>231</v>
       </c>
       <c r="L132" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="133" spans="1:14" ht="255" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B133" s="13" t="s">
         <v>237</v>
@@ -6725,13 +6742,13 @@
         <v>10</v>
       </c>
       <c r="G133" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H133" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I133" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J133" s="11" t="s">
         <v>230</v>
@@ -6740,13 +6757,13 @@
         <v>231</v>
       </c>
       <c r="L133" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M133" s="11"/>
     </row>
     <row r="134" spans="1:14" ht="255" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B134" s="13" t="s">
         <v>237</v>
@@ -6767,10 +6784,10 @@
         <v>259</v>
       </c>
       <c r="H134" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I134" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J134" s="11" t="s">
         <v>229</v>
@@ -6782,16 +6799,16 @@
         <v>231</v>
       </c>
       <c r="M134" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="N134" s="11"/>
     </row>
     <row r="135" spans="1:14" ht="135" x14ac:dyDescent="0.25">
-      <c r="A135" s="12" t="s">
+      <c r="A135" s="16" t="s">
         <v>277</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>237</v>
+        <v>369</v>
       </c>
       <c r="C135" t="s">
         <v>206</v>
@@ -6806,13 +6823,42 @@
         <v>10</v>
       </c>
       <c r="G135" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H135" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I135" s="11" t="s">
-        <v>278</v>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>370</v>
+      </c>
+      <c r="B136" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="C136" t="s">
+        <v>154</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G136" t="s">
+        <v>368</v>
+      </c>
+      <c r="H136" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="I136" s="11" t="s">
+        <v>371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Developed the test methods for date picker component
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_Merchant.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_Merchant.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COYNIv_2.3_Merchant\19-apr-2023(Merchant)\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2116D786-6FD5-494F-8EAB-25D404F42390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638B0C46-8C12-44B3-B5DA-443BB18D6143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="0" windowWidth="22665" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="379">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1083,26 +1084,6 @@
   </si>
   <si>
     <t>Verify Add Debit Card With Invalid Data</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>coyni_mobile_merchant.tests.MerchantProfileTest,
-testDebitCardWithInvalidData,
--pheading,
--paddPaymentHeading,
--pnameOnCard,
--pcardNumber,
--pcardExp,
--paddressLine1,
--paddressLine2,
--pcity,
--pstate,
--pzipCode,
--perrMsg,
--pelementName,
--pvalidateAddress</t>
   </si>
   <si>
     <t>coyni_mobile_merchant.tests.MerchantMenuIconTest,
@@ -2474,6 +2455,38 @@
 -ppassword,
 -pvalidateEmail,
 -pvalidatePassword</t>
+  </si>
+  <si>
+    <t>Verify Expired Debit Card in Withdraw Token and Payment Methods</t>
+  </si>
+  <si>
+    <t>coyni_mobile_merchant.tests.MerchantMenuIconTest,
+testWithdrawTokenWithExpiredDebitCard,
+-pselectWithdrawMethodHeading,
+-pwithdrawTokenHeading,
+-pwithdrawMethod,
+-pheading</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>coyni_mobile_merchant.tests.MerchantProfileTest,
+testDebitCardWithInvalidData,
+-pheading,
+-paddPaymentHeading,
+-pnameOnCard,
+-pcardNumber,
+-pcardExp,
+-paddressLine1,
+-paddressLine2,
+-pcity,
+-pstate,
+-pzipCode,
+-perrMsg,
+-pelementName,
+-pvalidateAddress,
+-pvalidatePopup</t>
   </si>
 </sst>
 </file>
@@ -2859,10 +2872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O138"/>
+  <dimension ref="A1:O139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B133" sqref="B133"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2913,30 +2926,30 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -2951,10 +2964,10 @@
         <v>10</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -2969,7 +2982,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -2999,10 +3012,10 @@
     </row>
     <row r="4" spans="1:15" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
@@ -3020,7 +3033,7 @@
         <v>26</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -3032,40 +3045,40 @@
     </row>
     <row r="5" spans="1:15" ht="345" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="J5" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>373</v>
-      </c>
-      <c r="I5" s="11" t="s">
+      <c r="K5" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="J5" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>229</v>
-      </c>
       <c r="L5" s="11" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="2"/>
@@ -3073,28 +3086,28 @@
     </row>
     <row r="6" spans="1:15" ht="375" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>370</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>372</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="C6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>374</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -3106,10 +3119,10 @@
     </row>
     <row r="7" spans="1:15" ht="330" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
@@ -3124,10 +3137,10 @@
         <v>10</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
@@ -3139,10 +3152,10 @@
     </row>
     <row r="8" spans="1:15" ht="102" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -3160,15 +3173,15 @@
         <v>11</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -3186,15 +3199,15 @@
         <v>11</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -3217,10 +3230,10 @@
     </row>
     <row r="11" spans="1:15" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -3238,15 +3251,15 @@
         <v>11</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -3264,7 +3277,7 @@
         <v>11</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="210" x14ac:dyDescent="0.25">
@@ -3272,7 +3285,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -3293,7 +3306,7 @@
         <v>18</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="210" x14ac:dyDescent="0.25">
@@ -3301,7 +3314,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -3324,10 +3337,10 @@
     </row>
     <row r="15" spans="1:15" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -3345,7 +3358,7 @@
         <v>17</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="195" x14ac:dyDescent="0.25">
@@ -3353,7 +3366,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C16" t="s">
         <v>29</v>
@@ -3379,7 +3392,7 @@
         <v>32</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C17" t="s">
         <v>29</v>
@@ -3405,7 +3418,7 @@
         <v>34</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C18" t="s">
         <v>29</v>
@@ -3431,7 +3444,7 @@
         <v>36</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C19" t="s">
         <v>29</v>
@@ -3454,10 +3467,10 @@
     </row>
     <row r="20" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C20" t="s">
         <v>29</v>
@@ -3475,7 +3488,7 @@
         <v>30</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -3483,7 +3496,7 @@
         <v>38</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
@@ -3509,7 +3522,7 @@
         <v>40</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -3527,7 +3540,7 @@
         <v>41</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="165" x14ac:dyDescent="0.25">
@@ -3535,7 +3548,7 @@
         <v>42</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -3553,7 +3566,7 @@
         <v>41</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -3561,7 +3574,7 @@
         <v>43</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C24" t="s">
         <v>16</v>
@@ -3587,7 +3600,7 @@
         <v>45</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C25" t="s">
         <v>46</v>
@@ -3605,7 +3618,7 @@
         <v>47</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I25" s="7" t="s">
         <v>48</v>
@@ -3616,7 +3629,7 @@
         <v>49</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C26" t="s">
         <v>46</v>
@@ -3634,7 +3647,7 @@
         <v>47</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I26" s="7" t="s">
         <v>50</v>
@@ -3642,10 +3655,10 @@
     </row>
     <row r="27" spans="1:9" ht="165.75" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C27" t="s">
         <v>46</v>
@@ -3663,10 +3676,10 @@
         <v>47</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="114.75" x14ac:dyDescent="0.25">
@@ -3674,7 +3687,7 @@
         <v>51</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C28" t="s">
         <v>46</v>
@@ -3692,7 +3705,7 @@
         <v>47</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I28" s="7" t="s">
         <v>52</v>
@@ -3703,7 +3716,7 @@
         <v>53</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C29" t="s">
         <v>54</v>
@@ -3721,18 +3734,18 @@
         <v>55</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="153" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C30" t="s">
         <v>54</v>
@@ -3750,10 +3763,10 @@
         <v>55</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="191.25" x14ac:dyDescent="0.25">
@@ -3761,7 +3774,7 @@
         <v>56</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C31" t="s">
         <v>54</v>
@@ -3779,7 +3792,7 @@
         <v>55</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I31" s="7" t="s">
         <v>58</v>
@@ -3790,7 +3803,7 @@
         <v>59</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C32" t="s">
         <v>54</v>
@@ -3808,7 +3821,7 @@
         <v>55</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I32" s="7" t="s">
         <v>60</v>
@@ -3819,7 +3832,7 @@
         <v>61</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C33" t="s">
         <v>62</v>
@@ -3837,19 +3850,19 @@
         <v>63</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J33" s="7"/>
     </row>
     <row r="34" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C34" t="s">
         <v>62</v>
@@ -3867,10 +3880,10 @@
         <v>63</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J34" s="7"/>
     </row>
@@ -3879,7 +3892,7 @@
         <v>64</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C35" t="s">
         <v>62</v>
@@ -3897,7 +3910,7 @@
         <v>63</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I35" s="7" t="s">
         <v>65</v>
@@ -3908,7 +3921,7 @@
         <v>66</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C36" t="s">
         <v>62</v>
@@ -3926,10 +3939,10 @@
         <v>63</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -3937,7 +3950,7 @@
         <v>67</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C37" t="s">
         <v>68</v>
@@ -3955,19 +3968,19 @@
         <v>69</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C38" t="s">
         <v>68</v>
@@ -3985,10 +3998,10 @@
         <v>69</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="J38" s="7"/>
     </row>
@@ -3997,7 +4010,7 @@
         <v>70</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C39" t="s">
         <v>68</v>
@@ -4015,7 +4028,7 @@
         <v>69</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I39" s="7" t="s">
         <v>71</v>
@@ -4026,7 +4039,7 @@
         <v>72</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C40" t="s">
         <v>68</v>
@@ -4044,18 +4057,18 @@
         <v>69</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="102" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C41" t="s">
         <v>68</v>
@@ -4073,10 +4086,10 @@
         <v>69</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="102" x14ac:dyDescent="0.25">
@@ -4084,7 +4097,7 @@
         <v>73</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C42" t="s">
         <v>74</v>
@@ -4102,10 +4115,10 @@
         <v>75</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="102" x14ac:dyDescent="0.25">
@@ -4113,7 +4126,7 @@
         <v>76</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C43" t="s">
         <v>74</v>
@@ -4131,7 +4144,7 @@
         <v>75</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I43" s="7" t="s">
         <v>77</v>
@@ -4142,7 +4155,7 @@
         <v>78</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C44" t="s">
         <v>79</v>
@@ -4160,7 +4173,7 @@
         <v>80</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I44" s="7" t="s">
         <v>81</v>
@@ -4168,10 +4181,10 @@
     </row>
     <row r="45" spans="1:10" ht="102" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C45" t="s">
         <v>79</v>
@@ -4189,10 +4202,10 @@
         <v>80</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
@@ -4200,7 +4213,7 @@
         <v>82</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C46" t="s">
         <v>79</v>
@@ -4218,10 +4231,10 @@
         <v>80</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="140.25" x14ac:dyDescent="0.25">
@@ -4229,7 +4242,7 @@
         <v>83</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C47" t="s">
         <v>79</v>
@@ -4247,7 +4260,7 @@
         <v>80</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I47" s="7" t="s">
         <v>84</v>
@@ -4258,7 +4271,7 @@
         <v>85</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C48" t="s">
         <v>79</v>
@@ -4276,7 +4289,7 @@
         <v>80</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I48" s="7" t="s">
         <v>86</v>
@@ -4284,10 +4297,10 @@
     </row>
     <row r="49" spans="1:9" ht="153" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C49" t="s">
         <v>79</v>
@@ -4305,10 +4318,10 @@
         <v>80</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="127.5" x14ac:dyDescent="0.25">
@@ -4316,7 +4329,7 @@
         <v>87</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C50" t="s">
         <v>79</v>
@@ -4334,10 +4347,10 @@
         <v>80</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="127.5" x14ac:dyDescent="0.25">
@@ -4345,7 +4358,7 @@
         <v>88</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C51" t="s">
         <v>79</v>
@@ -4363,7 +4376,7 @@
         <v>80</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I51" s="7" t="s">
         <v>89</v>
@@ -4374,7 +4387,7 @@
         <v>90</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C52" t="s">
         <v>79</v>
@@ -4392,7 +4405,7 @@
         <v>80</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I52" s="7" t="s">
         <v>91</v>
@@ -4403,7 +4416,7 @@
         <v>92</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C53" t="s">
         <v>93</v>
@@ -4421,7 +4434,7 @@
         <v>94</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I53" s="7" t="s">
         <v>95</v>
@@ -4432,7 +4445,7 @@
         <v>96</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C54" t="s">
         <v>93</v>
@@ -4450,10 +4463,10 @@
         <v>94</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="140.25" x14ac:dyDescent="0.25">
@@ -4461,7 +4474,7 @@
         <v>97</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C55" t="s">
         <v>93</v>
@@ -4479,7 +4492,7 @@
         <v>94</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I55" s="7" t="s">
         <v>98</v>
@@ -4490,7 +4503,7 @@
         <v>99</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C56" t="s">
         <v>93</v>
@@ -4508,7 +4521,7 @@
         <v>94</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I56" s="7" t="s">
         <v>100</v>
@@ -4516,10 +4529,10 @@
     </row>
     <row r="57" spans="1:9" ht="165.75" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C57" t="s">
         <v>93</v>
@@ -4537,10 +4550,10 @@
         <v>94</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="127.5" x14ac:dyDescent="0.25">
@@ -4548,7 +4561,7 @@
         <v>101</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C58" t="s">
         <v>93</v>
@@ -4566,10 +4579,10 @@
         <v>94</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="127.5" x14ac:dyDescent="0.25">
@@ -4577,7 +4590,7 @@
         <v>102</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C59" t="s">
         <v>93</v>
@@ -4595,7 +4608,7 @@
         <v>94</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I59" s="7" t="s">
         <v>103</v>
@@ -4606,7 +4619,7 @@
         <v>104</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C60" t="s">
         <v>93</v>
@@ -4624,7 +4637,7 @@
         <v>94</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I60" s="7" t="s">
         <v>105</v>
@@ -4635,7 +4648,7 @@
         <v>106</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C61" t="s">
         <v>107</v>
@@ -4653,7 +4666,7 @@
         <v>108</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I61" s="7" t="s">
         <v>109</v>
@@ -4664,7 +4677,7 @@
         <v>110</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C62" t="s">
         <v>107</v>
@@ -4682,7 +4695,7 @@
         <v>108</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I62" s="7" t="s">
         <v>111</v>
@@ -4693,7 +4706,7 @@
         <v>112</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C63" t="s">
         <v>113</v>
@@ -4711,10 +4724,10 @@
         <v>114</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I63" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="216.75" x14ac:dyDescent="0.25">
@@ -4722,7 +4735,7 @@
         <v>115</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C64" t="s">
         <v>113</v>
@@ -4740,7 +4753,7 @@
         <v>114</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I64" s="7" t="s">
         <v>117</v>
@@ -4751,7 +4764,7 @@
         <v>118</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C65" t="s">
         <v>113</v>
@@ -4769,7 +4782,7 @@
         <v>114</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I65" s="7" t="s">
         <v>119</v>
@@ -4777,10 +4790,10 @@
     </row>
     <row r="66" spans="1:9" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C66" t="s">
         <v>113</v>
@@ -4795,13 +4808,13 @@
         <v>10</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I66" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="204" x14ac:dyDescent="0.25">
@@ -4809,7 +4822,7 @@
         <v>120</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C67" t="s">
         <v>113</v>
@@ -4827,10 +4840,10 @@
         <v>121</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I67" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="242.25" x14ac:dyDescent="0.25">
@@ -4838,7 +4851,7 @@
         <v>122</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C68" t="s">
         <v>113</v>
@@ -4856,7 +4869,7 @@
         <v>121</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I68" s="7" t="s">
         <v>123</v>
@@ -4867,7 +4880,7 @@
         <v>124</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C69" t="s">
         <v>113</v>
@@ -4885,7 +4898,7 @@
         <v>121</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I69" s="7" t="s">
         <v>125</v>
@@ -4896,7 +4909,7 @@
         <v>126</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C70" t="s">
         <v>113</v>
@@ -4914,10 +4927,10 @@
         <v>127</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I70" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="102" x14ac:dyDescent="0.25">
@@ -4925,7 +4938,7 @@
         <v>128</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>129</v>
@@ -4943,7 +4956,7 @@
         <v>130</v>
       </c>
       <c r="H71" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I71" s="4" t="s">
         <v>131</v>
@@ -4954,7 +4967,7 @@
         <v>132</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>129</v>
@@ -4966,16 +4979,16 @@
         <v>10</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>133</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -4983,7 +4996,7 @@
         <v>134</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>129</v>
@@ -5001,7 +5014,7 @@
         <v>135</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I73" s="4" t="s">
         <v>136</v>
@@ -5012,7 +5025,7 @@
         <v>137</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>129</v>
@@ -5030,7 +5043,7 @@
         <v>138</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I74" s="4" t="s">
         <v>139</v>
@@ -5041,7 +5054,7 @@
         <v>140</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>129</v>
@@ -5059,7 +5072,7 @@
         <v>141</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I75" s="4" t="s">
         <v>142</v>
@@ -5067,10 +5080,10 @@
     </row>
     <row r="76" spans="1:9" ht="102" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C76" t="s">
         <v>152</v>
@@ -5085,21 +5098,21 @@
         <v>10</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="H76" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I76" s="11" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="102" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>144</v>
@@ -5117,10 +5130,10 @@
         <v>145</v>
       </c>
       <c r="H77" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -5128,7 +5141,7 @@
         <v>143</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>144</v>
@@ -5146,10 +5159,10 @@
         <v>145</v>
       </c>
       <c r="H78" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -5157,7 +5170,7 @@
         <v>146</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>144</v>
@@ -5175,7 +5188,7 @@
         <v>145</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I79" s="4" t="s">
         <v>147</v>
@@ -5186,7 +5199,7 @@
         <v>148</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>152</v>
@@ -5204,7 +5217,7 @@
         <v>149</v>
       </c>
       <c r="H80" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I80" s="4" t="s">
         <v>150</v>
@@ -5215,7 +5228,7 @@
         <v>151</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C81" t="s">
         <v>152</v>
@@ -5233,7 +5246,7 @@
         <v>153</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I81" s="11" t="s">
         <v>154</v>
@@ -5244,7 +5257,7 @@
         <v>155</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>152</v>
@@ -5262,7 +5275,7 @@
         <v>156</v>
       </c>
       <c r="H82" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I82" s="4" t="s">
         <v>157</v>
@@ -5273,7 +5286,7 @@
         <v>159</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C83" t="s">
         <v>152</v>
@@ -5291,7 +5304,7 @@
         <v>158</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I83" s="4" t="s">
         <v>160</v>
@@ -5299,10 +5312,10 @@
     </row>
     <row r="84" spans="1:9" ht="102" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C84" t="s">
         <v>152</v>
@@ -5320,10 +5333,10 @@
         <v>158</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="102" x14ac:dyDescent="0.25">
@@ -5331,7 +5344,7 @@
         <v>161</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C85" t="s">
         <v>152</v>
@@ -5349,7 +5362,7 @@
         <v>158</v>
       </c>
       <c r="H85" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I85" s="4" t="s">
         <v>162</v>
@@ -5357,10 +5370,10 @@
     </row>
     <row r="86" spans="1:9" ht="102" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C86" t="s">
         <v>152</v>
@@ -5378,10 +5391,10 @@
         <v>158</v>
       </c>
       <c r="H86" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="102" x14ac:dyDescent="0.25">
@@ -5389,7 +5402,7 @@
         <v>163</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>152</v>
@@ -5407,7 +5420,7 @@
         <v>164</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I87" s="4" t="s">
         <v>165</v>
@@ -5418,7 +5431,7 @@
         <v>166</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>152</v>
@@ -5436,7 +5449,7 @@
         <v>168</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I88" s="4" t="s">
         <v>169</v>
@@ -5447,7 +5460,7 @@
         <v>170</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>152</v>
@@ -5465,7 +5478,7 @@
         <v>171</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I89" s="4" t="s">
         <v>172</v>
@@ -5473,10 +5486,10 @@
     </row>
     <row r="90" spans="1:9" ht="102" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>152</v>
@@ -5494,18 +5507,18 @@
         <v>171</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="102" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>152</v>
@@ -5523,18 +5536,18 @@
         <v>171</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="102" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C92" t="s">
         <v>152</v>
@@ -5552,18 +5565,18 @@
         <v>174</v>
       </c>
       <c r="H92" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="102" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C93" t="s">
         <v>152</v>
@@ -5581,10 +5594,10 @@
         <v>174</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I93" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -5592,7 +5605,7 @@
         <v>173</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>235</v>
+        <v>364</v>
       </c>
       <c r="C94" t="s">
         <v>152</v>
@@ -5610,10 +5623,10 @@
         <v>174</v>
       </c>
       <c r="H94" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I94" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="375" x14ac:dyDescent="0.25">
@@ -5621,7 +5634,7 @@
         <v>175</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>235</v>
+        <v>364</v>
       </c>
       <c r="C95" t="s">
         <v>152</v>
@@ -5639,18 +5652,18 @@
         <v>174</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I95" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C96" t="s">
         <v>177</v>
@@ -5668,10 +5681,10 @@
         <v>178</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I96" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="97" spans="1:11" ht="165" x14ac:dyDescent="0.25">
@@ -5679,7 +5692,7 @@
         <v>176</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>235</v>
+        <v>364</v>
       </c>
       <c r="C97" t="s">
         <v>177</v>
@@ -5697,7 +5710,7 @@
         <v>178</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I97" s="4" t="s">
         <v>179</v>
@@ -5708,7 +5721,7 @@
         <v>180</v>
       </c>
       <c r="B98" s="13" t="s">
-        <v>235</v>
+        <v>364</v>
       </c>
       <c r="C98" t="s">
         <v>177</v>
@@ -5726,7 +5739,7 @@
         <v>178</v>
       </c>
       <c r="H98" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I98" s="4" t="s">
         <v>181</v>
@@ -5737,7 +5750,7 @@
         <v>182</v>
       </c>
       <c r="B99" s="13" t="s">
-        <v>235</v>
+        <v>364</v>
       </c>
       <c r="C99" t="s">
         <v>177</v>
@@ -5755,7 +5768,7 @@
         <v>178</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I99" s="4" t="s">
         <v>183</v>
@@ -5763,10 +5776,10 @@
     </row>
     <row r="100" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C100" t="s">
         <v>177</v>
@@ -5784,10 +5797,10 @@
         <v>178</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I100" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="101" spans="1:11" ht="102" x14ac:dyDescent="0.25">
@@ -5795,7 +5808,7 @@
         <v>184</v>
       </c>
       <c r="B101" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C101" t="s">
         <v>129</v>
@@ -5813,7 +5826,7 @@
         <v>185</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I101" s="4" t="s">
         <v>186</v>
@@ -5824,7 +5837,7 @@
         <v>187</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C102" t="s">
         <v>188</v>
@@ -5842,10 +5855,10 @@
         <v>189</v>
       </c>
       <c r="H102" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I102" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="103" spans="1:11" ht="195" x14ac:dyDescent="0.25">
@@ -5853,7 +5866,7 @@
         <v>190</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C103" t="s">
         <v>188</v>
@@ -5865,13 +5878,13 @@
         <v>10</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G103" t="s">
         <v>189</v>
       </c>
       <c r="H103" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I103" s="4" t="s">
         <v>191</v>
@@ -5882,7 +5895,7 @@
         <v>192</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C104" t="s">
         <v>188</v>
@@ -5900,7 +5913,7 @@
         <v>189</v>
       </c>
       <c r="H104" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I104" s="4" t="s">
         <v>193</v>
@@ -5908,10 +5921,10 @@
     </row>
     <row r="105" spans="1:11" ht="270" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C105" t="s">
         <v>204</v>
@@ -5926,13 +5939,13 @@
         <v>10</v>
       </c>
       <c r="G105" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="H105" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I105" s="11" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J105" s="11"/>
     </row>
@@ -5941,7 +5954,7 @@
         <v>196</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>195</v>
@@ -5959,10 +5972,10 @@
         <v>197</v>
       </c>
       <c r="H106" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I106" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="107" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
@@ -5970,7 +5983,7 @@
         <v>194</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C107" s="5" t="s">
         <v>195</v>
@@ -5985,24 +5998,24 @@
         <v>13</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H107" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I107" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="J107" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="108" spans="1:11" ht="270" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C108" t="s">
         <v>204</v>
@@ -6017,13 +6030,13 @@
         <v>10</v>
       </c>
       <c r="G108" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="H108" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I108" s="11" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J108" s="11"/>
     </row>
@@ -6032,7 +6045,7 @@
         <v>202</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C109" s="5" t="s">
         <v>199</v>
@@ -6047,13 +6060,13 @@
         <v>13</v>
       </c>
       <c r="G109" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H109" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I109" s="4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="110" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
@@ -6061,7 +6074,7 @@
         <v>198</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C110" s="5" t="s">
         <v>199</v>
@@ -6076,16 +6089,16 @@
         <v>13</v>
       </c>
       <c r="G110" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H110" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I110" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="J110" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="111" spans="1:11" ht="255" x14ac:dyDescent="0.25">
@@ -6093,7 +6106,7 @@
         <v>203</v>
       </c>
       <c r="B111" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C111" t="s">
         <v>204</v>
@@ -6108,23 +6121,23 @@
         <v>10</v>
       </c>
       <c r="G111" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H111" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I111" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J111" s="11"/>
       <c r="K111" s="11"/>
     </row>
     <row r="112" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B112" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C112" s="5" t="s">
         <v>199</v>
@@ -6139,22 +6152,22 @@
         <v>13</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H112" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I112" s="4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J112" s="11"/>
     </row>
-    <row r="113" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A113" s="5" t="s">
-        <v>350</v>
+    <row r="113" spans="1:11" ht="102" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>375</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C113" s="5" t="s">
         <v>199</v>
@@ -6169,22 +6182,22 @@
         <v>10</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H113" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I113" s="11" t="s">
-        <v>351</v>
+        <v>343</v>
+      </c>
+      <c r="I113" s="4" t="s">
+        <v>376</v>
       </c>
       <c r="J113" s="11"/>
     </row>
-    <row r="114" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>200</v>
+        <v>348</v>
       </c>
       <c r="B114" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C114" s="5" t="s">
         <v>199</v>
@@ -6196,87 +6209,87 @@
         <v>10</v>
       </c>
       <c r="F114" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G114" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="H114" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="I114" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="J114" s="11"/>
+    </row>
+    <row r="115" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B115" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E115" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F115" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G114" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="H114" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I114" s="11" t="s">
-        <v>327</v>
-      </c>
-      <c r="J114" s="11" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="115" spans="1:11" ht="225" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>265</v>
-      </c>
-      <c r="B115" s="13" t="s">
-        <v>366</v>
-      </c>
-      <c r="C115" t="s">
+      <c r="G115" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="H115" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="I115" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="J115" s="11" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>263</v>
+      </c>
+      <c r="B116" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C116" t="s">
         <v>204</v>
       </c>
-      <c r="D115" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F115" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G115" t="s">
-        <v>332</v>
-      </c>
-      <c r="H115" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I115" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="J115" s="11"/>
-    </row>
-    <row r="116" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="D116" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G116" t="s">
         <v>330</v>
       </c>
-      <c r="B116" s="13" t="s">
-        <v>366</v>
-      </c>
-      <c r="C116" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="D116" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E116" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F116" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G116" s="5" t="s">
-        <v>331</v>
-      </c>
       <c r="H116" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I116" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="J116" s="11"/>
+    </row>
+    <row r="117" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>328</v>
       </c>
-      <c r="J116" s="11"/>
-    </row>
-    <row r="117" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A117" s="5" t="s">
-        <v>348</v>
-      </c>
       <c r="B117" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C117" s="5" t="s">
         <v>199</v>
@@ -6288,25 +6301,25 @@
         <v>10</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G117" s="5" t="s">
-        <v>201</v>
+        <v>329</v>
       </c>
       <c r="H117" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I117" s="11" t="s">
-        <v>349</v>
+        <v>343</v>
+      </c>
+      <c r="I117" s="4" t="s">
+        <v>326</v>
       </c>
       <c r="J117" s="11"/>
     </row>
-    <row r="118" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>267</v>
+        <v>346</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>199</v>
@@ -6318,62 +6331,57 @@
         <v>10</v>
       </c>
       <c r="F118" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G118" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="H118" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="I118" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="J118" s="11"/>
+    </row>
+    <row r="119" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B119" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E119" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F119" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G118" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="H118" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I118" s="11" t="s">
-        <v>337</v>
-      </c>
-      <c r="J118" s="11" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11" ht="255" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="G119" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="H119" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="I119" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="J119" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" ht="255" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>203</v>
       </c>
-      <c r="B119" s="13" t="s">
-        <v>366</v>
-      </c>
-      <c r="C119" t="s">
-        <v>204</v>
-      </c>
-      <c r="D119" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E119" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F119" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G119" t="s">
-        <v>334</v>
-      </c>
-      <c r="H119" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I119" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="J119" s="11" t="s">
-        <v>352</v>
-      </c>
-      <c r="K119" s="11" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>277</v>
-      </c>
       <c r="B120" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C120" t="s">
         <v>204</v>
@@ -6388,23 +6396,27 @@
         <v>10</v>
       </c>
       <c r="G120" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H120" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I120" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="J120" s="11"/>
-      <c r="K120" s="11"/>
-    </row>
-    <row r="121" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+      <c r="J120" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="K120" s="11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>205</v>
+        <v>275</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C121" t="s">
         <v>204</v>
@@ -6416,24 +6428,26 @@
         <v>10</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>206</v>
+        <v>10</v>
       </c>
       <c r="G121" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H121" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I121" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+      <c r="J121" s="11"/>
+      <c r="K121" s="11"/>
+    </row>
+    <row r="122" spans="1:11" ht="240" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>265</v>
+        <v>205</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C122" t="s">
         <v>204</v>
@@ -6445,27 +6459,24 @@
         <v>10</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>10</v>
+        <v>377</v>
       </c>
       <c r="G122" t="s">
         <v>332</v>
       </c>
       <c r="H122" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I122" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="J122" s="11" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C123" t="s">
         <v>204</v>
@@ -6480,22 +6491,24 @@
         <v>10</v>
       </c>
       <c r="G123" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H123" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I123" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="J123" s="11"/>
-    </row>
-    <row r="124" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+      <c r="J123" s="11" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C124" t="s">
         <v>204</v>
@@ -6507,24 +6520,25 @@
         <v>10</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G124" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H124" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I124" s="4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11" ht="270" x14ac:dyDescent="0.25">
-      <c r="A125" s="14" t="s">
-        <v>304</v>
+        <v>278</v>
+      </c>
+      <c r="J124" s="11"/>
+    </row>
+    <row r="125" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>264</v>
       </c>
       <c r="B125" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C125" t="s">
         <v>204</v>
@@ -6536,27 +6550,24 @@
         <v>10</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="G125" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="H125" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I125" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="J125" s="11" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11" ht="165" x14ac:dyDescent="0.25">
-      <c r="A126" s="5" t="s">
-        <v>353</v>
+        <v>343</v>
+      </c>
+      <c r="I125" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" ht="270" x14ac:dyDescent="0.25">
+      <c r="A126" s="14" t="s">
+        <v>302</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C126" t="s">
         <v>204</v>
@@ -6571,22 +6582,24 @@
         <v>10</v>
       </c>
       <c r="G126" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="H126" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I126" s="11" t="s">
-        <v>355</v>
-      </c>
-      <c r="J126" s="11"/>
-    </row>
-    <row r="127" spans="1:11" ht="255" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>236</v>
+        <v>301</v>
+      </c>
+      <c r="J126" s="11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
+        <v>351</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C127" t="s">
         <v>204</v>
@@ -6598,24 +6611,25 @@
         <v>10</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>167</v>
+        <v>10</v>
       </c>
       <c r="G127" t="s">
-        <v>334</v>
+        <v>352</v>
       </c>
       <c r="H127" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I127" s="4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11" ht="102" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+      <c r="I127" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="J127" s="11"/>
+    </row>
+    <row r="128" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B128" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C128" t="s">
         <v>204</v>
@@ -6627,24 +6641,24 @@
         <v>10</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>10</v>
+        <v>167</v>
       </c>
       <c r="G128" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H128" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I128" s="11" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="129" spans="1:14" ht="225" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+      <c r="I128" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" ht="102" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>264</v>
+        <v>235</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C129" t="s">
         <v>204</v>
@@ -6656,24 +6670,24 @@
         <v>10</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>167</v>
+        <v>10</v>
       </c>
       <c r="G129" t="s">
         <v>332</v>
       </c>
       <c r="H129" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I129" s="4" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="130" spans="1:14" ht="102" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+      <c r="I129" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" ht="225" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>366</v>
+        <v>233</v>
       </c>
       <c r="C130" t="s">
         <v>204</v>
@@ -6685,25 +6699,24 @@
         <v>10</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>10</v>
+        <v>167</v>
       </c>
       <c r="G130" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H130" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I130" s="11" t="s">
-        <v>338</v>
-      </c>
-      <c r="J130" s="11"/>
-    </row>
-    <row r="131" spans="1:14" ht="210" x14ac:dyDescent="0.25">
-      <c r="A131" s="12" t="s">
-        <v>238</v>
+        <v>343</v>
+      </c>
+      <c r="I130" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" ht="102" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>261</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C131" t="s">
         <v>204</v>
@@ -6715,25 +6728,25 @@
         <v>10</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G131" t="s">
+        <v>330</v>
+      </c>
+      <c r="H131" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="I131" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="H131" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I131" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="J131" s="4"/>
-    </row>
-    <row r="132" spans="1:14" ht="102" x14ac:dyDescent="0.25">
+      <c r="J131" s="11"/>
+    </row>
+    <row r="132" spans="1:14" ht="210" x14ac:dyDescent="0.25">
       <c r="A132" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B132" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C132" t="s">
         <v>204</v>
@@ -6745,222 +6758,252 @@
         <v>10</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G132" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="H132" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I132" s="11" t="s">
-        <v>360</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="I132" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="J132" s="4"/>
     </row>
     <row r="133" spans="1:14" ht="102" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>254</v>
+      <c r="A133" s="12" t="s">
+        <v>237</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C133" t="s">
+        <v>204</v>
+      </c>
+      <c r="D133" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G133" t="s">
+        <v>334</v>
+      </c>
+      <c r="H133" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="I133" s="11" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" ht="102" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>252</v>
+      </c>
+      <c r="B134" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C134" t="s">
         <v>129</v>
       </c>
-      <c r="D133" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E133" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F133" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G133" t="s">
-        <v>341</v>
-      </c>
-      <c r="H133" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I133" s="11" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="134" spans="1:14" ht="255" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>313</v>
-      </c>
-      <c r="B134" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="C134" t="s">
-        <v>226</v>
-      </c>
       <c r="D134" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E134" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F134" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G134" s="5" t="s">
-        <v>319</v>
+      <c r="E134" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G134" t="s">
+        <v>339</v>
       </c>
       <c r="H134" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I134" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="J134" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="K134" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="L134" s="11" t="s">
-        <v>315</v>
+        <v>251</v>
       </c>
     </row>
     <row r="135" spans="1:14" ht="255" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C135" t="s">
+        <v>224</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E135" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F135" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G135" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="H135" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="I135" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="J135" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="D135" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E135" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F135" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G135" t="s">
-        <v>318</v>
-      </c>
-      <c r="H135" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I135" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="J135" s="11" t="s">
-        <v>228</v>
-      </c>
       <c r="K135" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="L135" s="11" t="s">
-        <v>315</v>
-      </c>
-      <c r="M135" s="11"/>
+        <v>313</v>
+      </c>
     </row>
     <row r="136" spans="1:14" ht="255" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C136" t="s">
+        <v>224</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G136" t="s">
+        <v>316</v>
+      </c>
+      <c r="H136" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="I136" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="J136" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="D136" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E136" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F136" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G136" t="s">
-        <v>257</v>
-      </c>
-      <c r="H136" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I136" s="11" t="s">
-        <v>320</v>
-      </c>
-      <c r="J136" s="11" t="s">
+      <c r="K136" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="K136" s="11" t="s">
-        <v>228</v>
-      </c>
       <c r="L136" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="M136" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="M136" s="11"/>
+    </row>
+    <row r="137" spans="1:14" ht="255" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>315</v>
       </c>
-      <c r="N136" s="11"/>
-    </row>
-    <row r="137" spans="1:14" ht="135" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>275</v>
-      </c>
       <c r="B137" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C137" t="s">
+        <v>224</v>
+      </c>
+      <c r="D137" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F137" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G137" t="s">
+        <v>255</v>
+      </c>
+      <c r="H137" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="I137" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="J137" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="K137" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="L137" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="M137" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="N137" s="11"/>
+    </row>
+    <row r="138" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>273</v>
+      </c>
+      <c r="B138" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C138" t="s">
         <v>204</v>
       </c>
-      <c r="D137" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E137" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F137" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G137" t="s">
-        <v>342</v>
-      </c>
-      <c r="H137" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I137" s="11" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="138" spans="1:14" ht="120" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>369</v>
-      </c>
-      <c r="B138" s="13" t="s">
+      <c r="D138" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F138" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G138" t="s">
+        <v>340</v>
+      </c>
+      <c r="H138" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="I138" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="C138" t="s">
+    </row>
+    <row r="139" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>367</v>
+      </c>
+      <c r="B139" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C139" t="s">
         <v>152</v>
       </c>
-      <c r="D138" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E138" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F138" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G138" t="s">
+      <c r="D139" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E139" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F139" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G139" t="s">
+        <v>363</v>
+      </c>
+      <c r="H139" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="I139" s="11" t="s">
         <v>365</v>
-      </c>
-      <c r="H138" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="I138" s="11" t="s">
-        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>